<commit_message>
ex142 updated: set sl offset as percent of channel width
</commit_message>
<xml_diff>
--- a/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
+++ b/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmral\AppData\Roaming\MetaQuotes\Terminal\36A64B8C79A6163D85E6173B54096685\MQL5\Experts\mq5ea\optimized_parameters\prop_challenge\ex142\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03BC3A6-D8E9-4A59-BD73-6ABB1D7D29BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE56A28-D907-4F5C-8F0A-66D4F9FDE141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="3036" windowWidth="22656" windowHeight="11856" xr2:uid="{BB71DF2C-F5C1-4051-9450-66D36914BD59}"/>
+    <workbookView xWindow="5016" yWindow="2940" windowWidth="22656" windowHeight="11856" xr2:uid="{BB71DF2C-F5C1-4051-9450-66D36914BD59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,11 +554,11 @@
         <f>D2/D3</f>
         <v>7.2758620689655169</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="1">
         <f t="shared" ref="J2:K2" si="0">E2/E3</f>
         <v>1.9163346613545817</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="11">
         <f t="shared" si="0"/>
         <v>-0.15</v>
       </c>
@@ -607,20 +607,20 @@
         <v>3</v>
       </c>
       <c r="C5" s="4">
-        <v>9921</v>
+        <v>13297</v>
       </c>
       <c r="D5" s="4">
         <v>2707</v>
       </c>
       <c r="E5" s="4">
-        <v>538</v>
+        <v>1348</v>
       </c>
       <c r="F5" s="4">
         <v>-801</v>
       </c>
       <c r="H5" s="1">
         <f>C5/C6</f>
-        <v>7.1891304347826086</v>
+        <v>9.4371894960965221</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5:K5" si="1">D5/D6</f>
@@ -628,9 +628,9 @@
       </c>
       <c r="J5" s="8">
         <f t="shared" si="1"/>
-        <v>0.76967095851216027</v>
-      </c>
-      <c r="K5" s="11">
+        <v>2.1228346456692915</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="1"/>
         <v>-1</v>
       </c>
@@ -641,13 +641,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="4">
-        <v>1380</v>
+        <v>1409</v>
       </c>
       <c r="D6" s="4">
         <v>1879</v>
       </c>
       <c r="E6" s="4">
-        <v>699</v>
+        <v>635</v>
       </c>
       <c r="F6" s="4">
         <v>801</v>
@@ -659,13 +659,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <v>1785</v>
+        <v>1831</v>
       </c>
       <c r="D7" s="4">
         <v>2381</v>
       </c>
       <c r="E7" s="4">
-        <v>1007</v>
+        <v>952</v>
       </c>
       <c r="F7" s="4">
         <v>903</v>
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="3">
-        <v>7575</v>
+        <v>8301</v>
       </c>
       <c r="D8" s="3">
         <v>5117</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="H8" s="1">
         <f>C8/C9</f>
-        <v>9.1818181818181817</v>
+        <v>10.273514851485148</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" ref="I8:K8" si="2">D8/D9</f>
@@ -702,7 +702,7 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="11">
         <f t="shared" si="2"/>
         <v>2184</v>
       </c>
@@ -713,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="3">
-        <v>825</v>
+        <v>808</v>
       </c>
       <c r="D9" s="3">
         <v>796</v>
@@ -731,7 +731,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="3">
-        <v>1249</v>
+        <v>1204</v>
       </c>
       <c r="D10" s="3">
         <v>1094</v>

</xml_diff>

<commit_message>
added spx500 for prop challenge
</commit_message>
<xml_diff>
--- a/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
+++ b/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmral\AppData\Roaming\MetaQuotes\Terminal\36A64B8C79A6163D85E6173B54096685\MQL5\Experts\mq5ea\optimized_parameters\prop_challenge\ex142\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE56A28-D907-4F5C-8F0A-66D4F9FDE141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AB3F4B-D93C-44FF-8453-8BCA2F6A1A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5016" yWindow="2940" windowWidth="22656" windowHeight="11856" xr2:uid="{BB71DF2C-F5C1-4051-9450-66D36914BD59}"/>
+    <workbookView xWindow="16644" yWindow="2544" windowWidth="22656" windowHeight="11856" xr2:uid="{BB71DF2C-F5C1-4051-9450-66D36914BD59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>EUR</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>mid 2022</t>
+  </si>
+  <si>
+    <t>SPX500 (2017-2022)</t>
   </si>
 </sst>
 </file>
@@ -494,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CA039F-A3B0-4469-8A78-93F2E9638520}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.109375" style="1" customWidth="1"/>
@@ -558,7 +561,7 @@
         <f t="shared" ref="J2:K2" si="0">E2/E3</f>
         <v>1.9163346613545817</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="1">
         <f t="shared" si="0"/>
         <v>-0.15</v>
       </c>
@@ -627,7 +630,7 @@
         <v>1.4406599254922832</v>
       </c>
       <c r="J5" s="8">
-        <f t="shared" si="1"/>
+        <f>E5/E6</f>
         <v>2.1228346456692915</v>
       </c>
       <c r="K5" s="1">
@@ -695,14 +698,14 @@
         <v>10.273514851485148</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:K8" si="2">D8/D9</f>
+        <f t="shared" ref="I8:K11" si="2">D8/D9</f>
         <v>6.4283919597989954</v>
       </c>
       <c r="J8" s="8" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="1">
         <f t="shared" si="2"/>
         <v>2184</v>
       </c>
@@ -724,6 +727,7 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
+      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
@@ -742,12 +746,66 @@
       <c r="F10" s="3">
         <v>441</v>
       </c>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4451</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4">
+        <v>69</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="H11" s="1">
+        <f t="shared" ref="H9:H11" si="3">C11/C12</f>
+        <v>6.2078103207810322</v>
+      </c>
+      <c r="J11" s="8">
+        <f>E11/E12</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4">
+        <v>717</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="4">
+        <v>912</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
+        <v>307</v>
+      </c>
+      <c r="F13" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
removed spx500 from prop challenge due to inconstintance results between spx500 and spx500_m
</commit_message>
<xml_diff>
--- a/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
+++ b/optimized_parameters/prop_challenge/ex142/reports/prop_challenge_15_to_31_jan_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmral\AppData\Roaming\MetaQuotes\Terminal\36A64B8C79A6163D85E6173B54096685\MQL5\Experts\mq5ea\optimized_parameters\prop_challenge\ex142\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AB3F4B-D93C-44FF-8453-8BCA2F6A1A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E46AEE-6194-4970-BAA5-6C33A84C0813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16644" yWindow="2544" windowWidth="22656" windowHeight="11856" xr2:uid="{BB71DF2C-F5C1-4051-9450-66D36914BD59}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,7 +698,7 @@
         <v>10.273514851485148</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ref="I8:K11" si="2">D8/D9</f>
+        <f t="shared" ref="I8:K8" si="2">D8/D9</f>
         <v>6.4283919597989954</v>
       </c>
       <c r="J8" s="8" t="e">
@@ -727,7 +727,6 @@
       <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="J9" s="11"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
@@ -746,7 +745,6 @@
       <c r="F10" s="3">
         <v>441</v>
       </c>
-      <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -764,10 +762,10 @@
       </c>
       <c r="F11" s="4"/>
       <c r="H11" s="1">
-        <f t="shared" ref="H9:H11" si="3">C11/C12</f>
+        <f t="shared" ref="H11" si="3">C11/C12</f>
         <v>6.2078103207810322</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="11">
         <f>E11/E12</f>
         <v>46</v>
       </c>

</xml_diff>